<commit_message>
finalised codebook D3_cohort_{ImmDis} including test
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -15,13 +15,12 @@
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
   <si>
     <t>status</t>
   </si>
@@ -116,21 +115,6 @@
     <t>SURVEY_ID VISIT_OCCURRENCE_ID</t>
   </si>
   <si>
-    <t>D3_clean_vaccines</t>
-  </si>
-  <si>
-    <t>01_T2_40_clean_vaccines</t>
-  </si>
-  <si>
-    <t>D3_vaccines_curated</t>
-  </si>
-  <si>
-    <t>01_T2_41_apply_criteria_for_doses</t>
-  </si>
-  <si>
-    <t>Flowchart_criteria_for_doses</t>
-  </si>
-  <si>
     <t>g_export</t>
   </si>
   <si>
@@ -182,50 +166,9 @@
     <t>04_itemsets</t>
   </si>
   <si>
-    <t>D3_all_vaccines_curated</t>
-  </si>
-  <si>
-    <t>01_T2_42_clean_all_vaccines</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conceptsetdataset</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>01_T2_43_curate_all_vaccines</t>
-  </si>
-  <si>
-    <t>D3_clean_all_vaccines</t>
-  </si>
-  <si>
-    <t>Flowchart_criteria_for_all_vaccines</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
-    <t>D3_clean_all_vaccines D3_vaccines_curated</t>
-  </si>
-  <si>
     <t>D3_TD_covariates_complete</t>
   </si>
   <si>
@@ -244,9 +187,6 @@
     <t>01_T2_60_selection_criteria_from_PERSON_to_source_population</t>
   </si>
   <si>
-    <t>D3_diagnoses_immune_diseases</t>
-  </si>
-  <si>
     <t>D3_components_flare_TD_E_GRAVES_AESI</t>
   </si>
   <si>
@@ -350,9 +290,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>first diagnosis of immune disease</t>
   </si>
   <si>
     <t>cohort of immune disease {ImmDis}, one record per person, repeated components</t>
@@ -441,36 +378,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D4_source_population</t>
-    </r>
-  </si>
-  <si>
-    <t>03_T2_10_create_diagnoses_of_immune_diseases</t>
-  </si>
-  <si>
-    <t>03_T2_30_create_components_flares</t>
-  </si>
-  <si>
-    <t>03_T2_20_create_cohort</t>
-  </si>
-  <si>
-    <t>03_T2_40_create_dates_flares</t>
-  </si>
-  <si>
-    <t>D3_diagnoses_immune_diseases D4_source_population</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">conceptsetdataset </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>D3_cohort_{ImmDis}</t>
     </r>
   </si>
@@ -493,9 +400,6 @@
     <t>03_T2_40_create_TD_datasets</t>
   </si>
   <si>
-    <t>03_T2_43_create_TD_covariates</t>
-  </si>
-  <si>
     <t>D4_persontime_{ImmDis}</t>
   </si>
   <si>
@@ -599,6 +503,47 @@
   </si>
   <si>
     <t>D5_data_KM_figure_{ImmDis}_masked</t>
+  </si>
+  <si>
+    <t>03_T2_10_create_cohort</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conceptsetdatasets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> D4_source_population D3_all_vaccines_curated</t>
+    </r>
+  </si>
+  <si>
+    <t>03_T2_20_create_components_flares</t>
+  </si>
+  <si>
+    <t>03_T2_30_create_dates_flares</t>
+  </si>
+  <si>
+    <t>03_T2_41_create_TD_covariates</t>
+  </si>
+  <si>
+    <t>D3_all_vaccine_dates</t>
+  </si>
+  <si>
+    <t>01_T2_10_ccollect_vaccine_dates</t>
   </si>
 </sst>
 </file>
@@ -1173,13 +1118,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1222,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1341,11 +1286,11 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>11</v>
@@ -1357,604 +1302,510 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>60</v>
+        <v>31</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="2"/>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="2"/>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>65</v>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>103</v>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>126</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>127</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>127</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" s="2"/>
+      <c r="E26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G27" s="2"/>
+      <c r="B27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" t="s">
         <v>114</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="144" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>140</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>142</v>
       </c>
-      <c r="D39" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>144</v>
       </c>
-      <c r="D41" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>145</v>
-      </c>
-      <c r="D43" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>164</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F44" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>163</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C19 B37:C1048576">
+  <conditionalFormatting sqref="B31:C1048576 B1:C13">
     <cfRule type="duplicateValues" dxfId="11" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
+  <conditionalFormatting sqref="F12">
     <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
+  <conditionalFormatting sqref="F11">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C30">
+  <conditionalFormatting sqref="B24:C24">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
+  <conditionalFormatting sqref="B25">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:C33">
+  <conditionalFormatting sqref="B26:C27">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
+  <conditionalFormatting sqref="F13">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
+  <conditionalFormatting sqref="F25">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
+  <conditionalFormatting sqref="F28">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
+  <conditionalFormatting sqref="F29">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
+  <conditionalFormatting sqref="F30">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D43">
+  <conditionalFormatting sqref="D32:D37">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1982,19 +1833,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2002,10 +1853,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2013,10 +1864,10 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2031,142 +1882,142 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" t="s">
-        <v>82</v>
-      </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2176,6 +2027,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2426,42 +2298,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2484,9 +2324,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
restored vaccine steps and codebooks
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="168">
   <si>
     <t>status</t>
   </si>
@@ -540,10 +540,75 @@
     <t>03_T2_41_create_TD_covariates</t>
   </si>
   <si>
-    <t>D3_all_vaccine_dates</t>
-  </si>
-  <si>
-    <t>01_T2_10_ccollect_vaccine_dates</t>
+    <t>who</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D/R</t>
+  </si>
+  <si>
+    <t>D3_clean_vaccines</t>
+  </si>
+  <si>
+    <t>01_T2_40_clean_vaccines</t>
+  </si>
+  <si>
+    <t>D3_vaccines_curated</t>
+  </si>
+  <si>
+    <t>01_T2_41_apply_criteria_for_doses</t>
+  </si>
+  <si>
+    <t>D3_clean_all_vaccines</t>
+  </si>
+  <si>
+    <t>01_T2_42_clean_all_vaccines</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conceptsetdataset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>D3_all_vaccines_curated</t>
+  </si>
+  <si>
+    <t>01_T2_43_curate_all_vaccines</t>
+  </si>
+  <si>
+    <t>D3_clean_all_vaccines D3_vaccines_curated</t>
+  </si>
+  <si>
+    <t>D5_Flowchart_criteria_for_all_vaccines</t>
+  </si>
+  <si>
+    <t>D5_Flowchart_criteria_for_doses</t>
   </si>
 </sst>
 </file>
@@ -615,7 +680,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,6 +699,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -647,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -676,18 +753,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -810,6 +899,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1118,694 +1212,934 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.6640625" customWidth="1"/>
-    <col min="3" max="3" width="52.88671875" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="86.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.88671875" customWidth="1"/>
+    <col min="5" max="5" width="46.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="86.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="14" t="s">
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>165</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="G14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="15" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="F16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="G16" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D19" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D20" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" t="s">
         <v>79</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D21" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" t="s">
         <v>81</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D22" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D23" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D24" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D25" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
         <v>85</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D26" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D27" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B28" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
         <v>87</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D28" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="G34" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+    <row r="35" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
         <v>120</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" t="s">
         <v>121</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E38" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" t="s">
         <v>122</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E39" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s">
         <v>123</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E40" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" t="s">
         <v>126</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E41" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" t="s">
         <v>124</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E42" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G43" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" t="s">
         <v>142</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G44" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C54" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B31:C1048576 B1:C13">
-    <cfRule type="duplicateValues" dxfId="11" priority="15"/>
+  <conditionalFormatting sqref="C36:D1048576 C1:D7 C14:D18">
+    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
+  <conditionalFormatting sqref="G17">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
     <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="C29:D29">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:C24">
+  <conditionalFormatting sqref="C30">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
+  <conditionalFormatting sqref="C31:D32">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:C27">
+  <conditionalFormatting sqref="G18">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="G30">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
+  <conditionalFormatting sqref="G33">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
+  <conditionalFormatting sqref="G34">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
+  <conditionalFormatting sqref="G35">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30">
+  <conditionalFormatting sqref="E37:E42">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32:D37">
+  <conditionalFormatting sqref="C8:C13">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2027,27 +2361,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2298,10 +2611,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2324,20 +2669,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated codebook D3_cohort_{ImmDis}, example still undergoing update
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="169">
   <si>
     <t>status</t>
   </si>
@@ -609,6 +609,9 @@
   </si>
   <si>
     <t>D5_Flowchart_criteria_for_doses</t>
+  </si>
+  <si>
+    <t>03_T2_50_create_periods_followup</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1218,10 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,35 +1801,46 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>109</v>
-      </c>
+      <c r="B30" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>105</v>
+      <c r="C31" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="15" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>38</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
@@ -1837,27 +1851,23 @@
       <c r="L31" s="14"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="14"/>
+      <c r="B32" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="I32" s="14"/>
-      <c r="J32" s="14" t="s">
-        <v>39</v>
-      </c>
+      <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
     </row>
@@ -2104,42 +2114,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C36:D1048576 C1:D7 C14:D18">
-    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:D29">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:D32">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="C30:D31">
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
+    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
+  <conditionalFormatting sqref="G34">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
+  <conditionalFormatting sqref="G35">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
+  <conditionalFormatting sqref="E37:E42">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
+  <conditionalFormatting sqref="C8:C13">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37:E42">
+  <conditionalFormatting sqref="C32">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C13">
+  <conditionalFormatting sqref="G32">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2361,6 +2371,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2611,18 +2633,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2633,6 +2643,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2651,23 +2678,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
first complete draft of index
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="182">
   <si>
     <t>status</t>
   </si>
@@ -133,9 +133,6 @@
     <t>g_output</t>
   </si>
   <si>
-    <t>Flowchart_exclusion_criteria</t>
-  </si>
-  <si>
     <t>g_intermediate/TD</t>
   </si>
   <si>
@@ -323,9 +320,6 @@
   </si>
   <si>
     <t>time-dependent components of flares for D_HEPATITISAUTOIMMUNE_AESI</t>
-  </si>
-  <si>
-    <t>dates of flares of {ImmDis}, label includes component status</t>
   </si>
   <si>
     <t>D3_followup_periods_in_cohort_{ImmDis}</t>
@@ -358,6 +352,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>condition</t>
@@ -409,19 +404,7 @@
     <t>D4_analytical_dataset_KM_{ImmDis}</t>
   </si>
   <si>
-    <t>D4_components_{ImmDis}</t>
-  </si>
-  <si>
-    <t>04_T3_20_create_components_dataset</t>
-  </si>
-  <si>
-    <t>04_T3_30_create_analytical_dataset_KM</t>
-  </si>
-  <si>
     <t>D3_followup_periods_in_cohort_{ImmDis} D3_flares_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D3_cohort_{ImmDis} D3_flares_{ImmDis}</t>
   </si>
   <si>
     <t>D5_Table_1_Attrition_{ImmDis}</t>
@@ -613,12 +596,69 @@
   <si>
     <t>03_T2_50_create_periods_followup</t>
   </si>
+  <si>
+    <t>dates of flares of {ImmDis}</t>
+  </si>
+  <si>
+    <t>04_T3_20_create_analytical_dataset_KM</t>
+  </si>
+  <si>
+    <t>04_T3_30_create_components_dataset</t>
+  </si>
+  <si>
+    <t>D4_components_flare_E_GRAVES_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_Im_HASHIMOTO_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_V_PAN_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_TD_M_ARTRHEU_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_TD_M_ARTPSORIATIC_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_N_DEMYELMS_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_SK_ERYTHEMANODOSUM_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_Im_SLE_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_D_ULCERATIVECOLITIS_AESI</t>
+  </si>
+  <si>
+    <t>D4_components_flare_D_HEPATITISAUTOIMMUNE_AESI</t>
+  </si>
+  <si>
+    <t>analytical dataset for component strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3_components_flare_TD_E_GRAVES_AESI D3_components_flare_TD_Im_HASHIMOTO_AESI D3_components_flare_TD_V_PAN_AESI D3_components_flare_TD_M_ARTRHEU_AESI D3_components_flare_TD_M_ARTPSORIATIC_AESI D3_components_flare_TD_N_DEMYELMS_AESI D3_components_flare_TD_SK_ERYTHEMANODOSUM_AESI D3_components_flare_TD_Im_SLE_AESI D3_components_flare_TD_D_ULCERATIVECOLITIS_AESI D3_components_flare_TD_D_HEPATITISAUTOIMMUNE_AESI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4_components_flare_E_GRAVES_AESI D4_components_flare_Im_HASHIMOTO_AESI D4_components_flare_V_PAN_AESI D4_components_flare_TD_M_ARTRHEU_AESI D4_components_flare_TD_M_ARTPSORIATIC_AESI D4_components_flare_N_DEMYELMS_AESI D4_components_flare_SK_ERYTHEMANODOSUM_AESI D4_components_flare_Im_SLE_AESI D4_components_flare_D_ULCERATIVECOLITIS_AESI D4_components_flare_D_HEPATITISAUTOIMMUNE_AESI </t>
+  </si>
+  <si>
+    <t>D5_Flowchart_exclusion_criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5_Flowchart_exclusion_criteria D3_cohort_{ImmDis} </t>
+  </si>
+  <si>
+    <t>D3_cohort_{ImmDis} D3_TD_covariates_complete</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,11 +694,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -666,6 +708,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -674,13 +717,6 @@
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -761,25 +797,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1215,13 +1241,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1240,13 +1266,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1267,7 +1293,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1275,7 +1301,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
@@ -1293,7 +1319,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>13</v>
@@ -1314,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>15</v>
@@ -1335,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>19</v>
@@ -1397,14 +1423,14 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
-        <v>153</v>
+      <c r="B8" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -1416,101 +1442,101 @@
       <c r="I8"/>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>153</v>
+      <c r="B11" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
-        <v>153</v>
+      <c r="B12" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
-        <v>153</v>
+      <c r="B13" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F13" t="s">
         <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>32</v>
@@ -1529,14 +1555,14 @@
     </row>
     <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>11</v>
@@ -1548,215 +1574,215 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E20" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
         <v>81</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E23" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" t="s">
         <v>82</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E24" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" t="s">
         <v>83</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E25" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" t="s">
         <v>84</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E26" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" t="s">
         <v>85</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" t="s">
-        <v>99</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -1764,393 +1790,567 @@
       <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>153</v>
+      <c r="B28" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>153</v>
+      <c r="B29" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="15" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K31" s="14"/>
       <c r="L31" s="14"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E34" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="G33" s="10" t="s">
+    </row>
+    <row r="35" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B35" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B36" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B37" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" t="s">
+        <v>176</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B38" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B39" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B41" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B42" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B43" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B44" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" t="s">
+        <v>175</v>
+      </c>
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" t="s">
+        <v>132</v>
+      </c>
+      <c r="G47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" t="s">
+        <v>133</v>
+      </c>
+      <c r="G48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G34" s="10" t="s">
+      <c r="E49" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E51" t="s">
+        <v>134</v>
+      </c>
+      <c r="G51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C37" t="s">
-        <v>120</v>
-      </c>
-      <c r="E37" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="E54" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" t="s">
         <v>121</v>
       </c>
-      <c r="E38" t="s">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" t="s">
-        <v>122</v>
-      </c>
-      <c r="E39" t="s">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" t="s">
-        <v>123</v>
-      </c>
-      <c r="E40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C42" t="s">
-        <v>124</v>
-      </c>
-      <c r="E42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C43" t="s">
-        <v>143</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" t="s">
-        <v>142</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C55" t="s">
-        <v>145</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C36:D1048576 C1:D7 C14:D18">
-    <cfRule type="duplicateValues" dxfId="12" priority="18"/>
+  <conditionalFormatting sqref="C45:D69 C1:D7 C14:D18 C80:D1048576 D70:D79">
+    <cfRule type="duplicateValues" dxfId="11" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:D29">
-    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:D31">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37:E42">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="E46:E51">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33 G35:G44">
+    <cfRule type="duplicateValues" dxfId="0" priority="23"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2177,19 +2377,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2197,10 +2397,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2208,10 +2408,10 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
         <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,142 +2426,142 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
         <v>68</v>
       </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
         <v>70</v>
       </c>
-      <c r="C12" t="s">
-        <v>71</v>
-      </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
         <v>76</v>
       </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2371,18 +2571,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2633,6 +2821,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2643,23 +2843,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2678,6 +2861,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updated documentation and remove curly bracket in dataset names
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20414"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18_Objective_2\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18_Objective_2\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901BF20D-B922-43EA-97B6-459D1BB98CFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="142">
   <si>
     <t>status</t>
   </si>
@@ -169,9 +170,6 @@
     <t>D3_TD_covariates_complete</t>
   </si>
   <si>
-    <t>D3_cohort_{ImmDis}</t>
-  </si>
-  <si>
     <t>D4_source_population</t>
   </si>
   <si>
@@ -184,9 +182,6 @@
     <t>01_T2_60_selection_criteria_from_PERSON_to_source_population</t>
   </si>
   <si>
-    <t>D3_components_flare_TD_E_GRAVES_AESI</t>
-  </si>
-  <si>
     <t>ImmDis</t>
   </si>
   <si>
@@ -256,73 +251,7 @@
     <t>label</t>
   </si>
   <si>
-    <t>D3_components_flare_TD_V_PAN_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_Im_HASHIMOTO_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_M_ARTRHEU_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_M_ARTPSORIATIC_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_N_DEMYELMS_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_SK_ERYTHEMANODOSUM_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_Im_SLE_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_D_ULCERATIVECOLITIS_AESI</t>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_D_HEPATITISAUTOIMMUNE_AESI</t>
-  </si>
-  <si>
-    <t>D3_flares_{ImmDis}</t>
-  </si>
-  <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>cohort of immune disease {ImmDis}, one record per person, repeated components</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for E_GRAVES_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for Im_HASHIMOTO_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for V_PAN_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for M_ARTRHEU_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for M_ARTPSORIATIC_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for N_DEMYELMS_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for SK_ERYTHEMANODOSUM_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for  Im_SLE_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for D_ULCERATIVECOLITIS_AESI</t>
-  </si>
-  <si>
-    <t>time-dependent components of flares for D_HEPATITISAUTOIMMUNE_AESI</t>
-  </si>
-  <si>
-    <t>D3_followup_periods_in_cohort_{ImmDis}</t>
   </si>
   <si>
     <t>D4_source_population conceptsetdataset</t>
@@ -362,99 +291,12 @@
     <t>multiple rows per person, split according to vaccinations and/or flares</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">conceptsetdataset </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D3_cohort_{ImmDis}</t>
-    </r>
-  </si>
-  <si>
-    <t>D3_components_flare_TD_E_GRAVES_AESI
-D3_components_flare_TD_Im_HASHIMOTO_AESI
-D3_components_flare_TD_V_PAN_AESI
-D3_components_flare_TD_M_ARTRHEU_AESI
-D3_components_flare_TD_M_ARTPSORIATIC_AESI
-D3_components_flare_TD_N_DEMYELMS_AESI
-D3_components_flare_TD_SK_ERYTHEMANODOSUM_AESI
-D3_components_flare_TD_Im_SLE_AESI
-D3_components_flare_TD_D_ULCERATIVECOLITIS_AESI
-D3_components_flare_TD_D_HEPATITISAUTOIMMUNE_AESI</t>
-  </si>
-  <si>
-    <t>D3_flares_{ImmDis} D3_all_vaccines_curated D3_cohort_{ImmDis}</t>
-  </si>
-  <si>
     <t>03_T2_40_create_TD_datasets</t>
   </si>
   <si>
-    <t>D4_persontime_{ImmDis}</t>
-  </si>
-  <si>
     <t>04_T3_10_create_persontime</t>
   </si>
   <si>
-    <t>D4_analytical_dataset_KM_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D3_followup_periods_in_cohort_{ImmDis} D3_flares_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_1_Attrition_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_2_Cohort_characteristics_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_3_Covariates_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_4_IR_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_5_IR_{ImmDis}_{stratum}</t>
-  </si>
-  <si>
-    <t>D5_Table_6_components_flares_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_8_components_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Histogram_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_1_Attrition_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_Table_2_Cohort_characteristics_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_Table_3_Covariates_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_Table_4_IR_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_Table_5_IR_{ImmDis}_{stratum}_masked</t>
-  </si>
-  <si>
-    <t>D5_Table_6_components_flares_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_Table_8_components_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_Histogram_{ImmDis}_masked</t>
-  </si>
-  <si>
     <t>05_T4_60_KM_analysis</t>
   </si>
   <si>
@@ -470,48 +312,10 @@
     <t>05_T4_40_Table_4_5_IR</t>
   </si>
   <si>
-    <t>05_T4_50_Table_6_components_flares_{ImmDis}</t>
-  </si>
-  <si>
     <t>05_T4_70_component_stategy</t>
   </si>
   <si>
-    <t>D5_data_KM_figure_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_7_cumulative_incidence_{ImmDis}</t>
-  </si>
-  <si>
-    <t>D5_Table_7_cumulative_incidence_{ImmDis}_masked</t>
-  </si>
-  <si>
-    <t>D5_data_KM_figure_{ImmDis}_masked</t>
-  </si>
-  <si>
     <t>03_T2_10_create_cohort</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conceptsetdatasets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> D4_source_population D3_all_vaccines_curated</t>
-    </r>
   </si>
   <si>
     <t>03_T2_20_create_components_flares</t>
@@ -597,67 +401,123 @@
     <t>03_T2_50_create_periods_followup</t>
   </si>
   <si>
-    <t>dates of flares of {ImmDis}</t>
-  </si>
-  <si>
     <t>04_T3_20_create_analytical_dataset_KM</t>
   </si>
   <si>
     <t>04_T3_30_create_components_dataset</t>
   </si>
   <si>
-    <t>D4_components_flare_E_GRAVES_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_Im_HASHIMOTO_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_V_PAN_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_TD_M_ARTRHEU_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_TD_M_ARTPSORIATIC_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_N_DEMYELMS_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_SK_ERYTHEMANODOSUM_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_Im_SLE_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_D_ULCERATIVECOLITIS_AESI</t>
-  </si>
-  <si>
-    <t>D4_components_flare_D_HEPATITISAUTOIMMUNE_AESI</t>
-  </si>
-  <si>
     <t>analytical dataset for component strategy</t>
   </si>
   <si>
-    <t xml:space="preserve">D3_components_flare_TD_E_GRAVES_AESI D3_components_flare_TD_Im_HASHIMOTO_AESI D3_components_flare_TD_V_PAN_AESI D3_components_flare_TD_M_ARTRHEU_AESI D3_components_flare_TD_M_ARTPSORIATIC_AESI D3_components_flare_TD_N_DEMYELMS_AESI D3_components_flare_TD_SK_ERYTHEMANODOSUM_AESI D3_components_flare_TD_Im_SLE_AESI D3_components_flare_TD_D_ULCERATIVECOLITIS_AESI D3_components_flare_TD_D_HEPATITISAUTOIMMUNE_AESI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">D4_components_flare_E_GRAVES_AESI D4_components_flare_Im_HASHIMOTO_AESI D4_components_flare_V_PAN_AESI D4_components_flare_TD_M_ARTRHEU_AESI D4_components_flare_TD_M_ARTPSORIATIC_AESI D4_components_flare_N_DEMYELMS_AESI D4_components_flare_SK_ERYTHEMANODOSUM_AESI D4_components_flare_Im_SLE_AESI D4_components_flare_D_ULCERATIVECOLITIS_AESI D4_components_flare_D_HEPATITISAUTOIMMUNE_AESI </t>
-  </si>
-  <si>
     <t>D5_Flowchart_exclusion_criteria</t>
   </si>
   <si>
-    <t xml:space="preserve">D5_Flowchart_exclusion_criteria D3_cohort_{ImmDis} </t>
-  </si>
-  <si>
-    <t>D3_cohort_{ImmDis} D3_TD_covariates_complete</t>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conceptsetdataset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> D4_source_population D3_all_vaccines_curated</t>
+    </r>
+  </si>
+  <si>
+    <t>D3_cohort_ImmDis</t>
+  </si>
+  <si>
+    <t>cohort of immune disease ImmDis, one record per person, repeated components</t>
+  </si>
+  <si>
+    <t>D3_components_flare_TD_ImmDis</t>
+  </si>
+  <si>
+    <t>time-dependent components of flares for ImmDis</t>
+  </si>
+  <si>
+    <t>conceptsetdataset D3_cohort_ImmDis</t>
+  </si>
+  <si>
+    <t>D3_flares_ImmDis</t>
+  </si>
+  <si>
+    <t>dates of flares of ImmDis</t>
+  </si>
+  <si>
+    <t>D3_followup_periods_in_cohort_ImmDis</t>
+  </si>
+  <si>
+    <t>D3_flares_ImmDis D3_all_vaccines_curated D3_cohort_ImmDis D4_source_population</t>
+  </si>
+  <si>
+    <t>D4_persontime_ImmDis</t>
+  </si>
+  <si>
+    <t>D3_followup_periods_in_cohort_ImmDis D3_flares_ImmDis</t>
+  </si>
+  <si>
+    <t>D4_analytical_dataset_KM_ImmDis</t>
+  </si>
+  <si>
+    <t>D4_components_flare_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_1_Attrition_ImmDis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5_Flowchart_exclusion_criteria D3_cohort_ImmDis </t>
+  </si>
+  <si>
+    <t>D5_Table_2_Cohort_characteristics_ImmDis</t>
+  </si>
+  <si>
+    <t>D3_cohort_ImmDis D3_TD_covariates_complete</t>
+  </si>
+  <si>
+    <t>D5_Table_3_Covariates_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_4_IR_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Histogram_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_6_components_flares_ImmDis</t>
+  </si>
+  <si>
+    <t>05_T4_50_Table_6_components_flares_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_7_cumulative_incidence_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_data_KM_figure_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_8_components_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_5_IR_ImmDis_stratum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -803,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1240,39 +1100,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G54" sqref="G54"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.6640625" customWidth="1"/>
-    <col min="4" max="4" width="52.88671875" customWidth="1"/>
-    <col min="5" max="5" width="46.5546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="86.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="86.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1296,12 +1156,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
@@ -1317,9 +1177,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>13</v>
@@ -1335,12 +1195,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>15</v>
@@ -1356,12 +1216,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>19</v>
@@ -1380,7 +1240,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1401,7 +1261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1422,15 +1282,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -1441,102 +1301,102 @@
       <c r="H8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>152</v>
+        <v>100</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
         <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>32</v>
@@ -1553,16 +1413,16 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>11</v>
@@ -1572,785 +1432,390 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>179</v>
+        <v>114</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="G18" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" t="s">
         <v>140</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B35" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B36" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" t="s">
-        <v>167</v>
-      </c>
-      <c r="D36" t="s">
-        <v>176</v>
-      </c>
       <c r="E36" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B37" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C37" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B38" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" t="s">
-        <v>176</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B39" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" t="s">
-        <v>176</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B40" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C40" t="s">
-        <v>171</v>
-      </c>
-      <c r="D40" t="s">
-        <v>176</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B41" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" t="s">
-        <v>176</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B42" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C42" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" t="s">
-        <v>176</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B43" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" t="s">
-        <v>176</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B44" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C44" t="s">
-        <v>175</v>
-      </c>
-      <c r="D44" t="s">
-        <v>176</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C45" t="s">
-        <v>113</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" t="s">
-        <v>131</v>
-      </c>
-      <c r="G46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" t="s">
-        <v>115</v>
-      </c>
-      <c r="E47" t="s">
-        <v>132</v>
-      </c>
-      <c r="G47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" t="s">
         <v>116</v>
       </c>
-      <c r="E48" t="s">
-        <v>133</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C49" t="s">
-        <v>117</v>
-      </c>
-      <c r="E49" t="s">
-        <v>133</v>
-      </c>
-      <c r="G49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C50" t="s">
-        <v>120</v>
-      </c>
-      <c r="E50" t="s">
-        <v>133</v>
-      </c>
-      <c r="G50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C51" t="s">
-        <v>118</v>
-      </c>
-      <c r="E51" t="s">
-        <v>134</v>
-      </c>
-      <c r="G51" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" t="s">
-        <v>137</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C53" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" t="s">
-        <v>119</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G54" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C55" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C56" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C58" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C59" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C61" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C62" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C64" t="s">
-        <v>139</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C45:D69 C1:D7 C14:D18 C80:D1048576 D70:D79">
-    <cfRule type="duplicateValues" dxfId="11" priority="18"/>
+  <conditionalFormatting sqref="C52:D1048576 C1:D7 C14:D18 D42:D51 C27:D41">
+    <cfRule type="duplicateValues" dxfId="11" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:D29">
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+  <conditionalFormatting sqref="C20:D20">
+    <cfRule type="duplicateValues" dxfId="8" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:D31">
-    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
+  <conditionalFormatting sqref="C21:D22">
+    <cfRule type="duplicateValues" dxfId="7" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  <conditionalFormatting sqref="G25">
+    <cfRule type="duplicateValues" dxfId="5" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46:E51">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="E28:E33">
+    <cfRule type="duplicateValues" dxfId="4" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33 G35:G44">
-    <cfRule type="duplicateValues" dxfId="0" priority="23"/>
+  <conditionalFormatting sqref="G24 G26">
+    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2358,7 +1823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2368,14 +1833,14 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -2383,7 +1848,7 @@
         <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>41</v>
@@ -2392,7 +1857,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2403,7 +1868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2414,154 +1879,154 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>72</v>
       </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>76</v>
-      </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2571,6 +2036,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2821,7 +2295,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -2833,16 +2307,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2861,7 +2334,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2876,12 +2349,4 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
minor modifications to index
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18_Objective_2\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18_Objective_2\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901BF20D-B922-43EA-97B6-459D1BB98CFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="144">
   <si>
     <t>status</t>
   </si>
@@ -448,9 +447,6 @@
     <t>time-dependent components of flares for ImmDis</t>
   </si>
   <si>
-    <t>conceptsetdataset D3_cohort_ImmDis</t>
-  </si>
-  <si>
     <t>D3_flares_ImmDis</t>
   </si>
   <si>
@@ -496,28 +492,49 @@
     <t>D5_Histogram_ImmDis</t>
   </si>
   <si>
-    <t>D5_Table_6_components_flares_ImmDis</t>
-  </si>
-  <si>
-    <t>05_T4_50_Table_6_components_flares_ImmDis</t>
-  </si>
-  <si>
     <t>D5_Table_7_cumulative_incidence_ImmDis</t>
   </si>
   <si>
     <t>D5_data_KM_figure_ImmDis</t>
   </si>
   <si>
-    <t>D5_Table_8_components_ImmDis</t>
-  </si>
-  <si>
     <t>D5_Table_5_IR_ImmDis_stratum</t>
+  </si>
+  <si>
+    <t>D3_followup_periods_in_cohort_ImmDis D3_PERSONS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">conceptsetdataset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D3_cohort_ImmDis</t>
+    </r>
+  </si>
+  <si>
+    <t>05_T4_50_Table_6_components_flares_{ImmDis}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4_components_flare_E_GRAVES_AESI D4_components_flare_Im_HASHIMOTO_AESI D4_components_flare_V_PAN_AESI D4_components_flare_TD_M_ARTRHEU_AESI D4_components_flare_TD_M_ARTPSORIATIC_AESI D4_components_flare_N_DEMYELMS_AESI D4_components_flare_SK_ERYTHEMANODOSUM_AESI D4_components_flare_Im_SLE_AESI D4_components_flare_D_ULCERATIVECOLITIS_AESI D4_components_flare_D_HEPATITISAUTOIMMUNE_AESI </t>
+  </si>
+  <si>
+    <t>D5_Table_6_Impact_of_component_flare_ImmDis</t>
+  </si>
+  <si>
+    <t>D5_Table_8_Impact_of_ablation_cohort_ImmDis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -663,9 +680,59 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1100,28 +1167,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
-    <col min="7" max="7" width="86.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.88671875" customWidth="1"/>
+    <col min="5" max="5" width="46.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="86.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1156,7 +1223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1177,7 +1244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>94</v>
       </c>
@@ -1195,7 +1262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1216,7 +1283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1240,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1261,7 +1328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1282,7 +1349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>95</v>
       </c>
@@ -1301,7 +1368,7 @@
       <c r="H8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>95</v>
       </c>
@@ -1320,7 +1387,7 @@
       <c r="H9"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>95</v>
       </c>
@@ -1339,7 +1406,7 @@
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>95</v>
       </c>
@@ -1358,7 +1425,7 @@
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>95</v>
       </c>
@@ -1377,7 +1444,7 @@
       <c r="H12"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>95</v>
       </c>
@@ -1394,7 +1461,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>94</v>
       </c>
@@ -1413,7 +1480,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>94</v>
       </c>
@@ -1432,7 +1499,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>94</v>
       </c>
@@ -1451,7 +1518,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>94</v>
       </c>
@@ -1470,7 +1537,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>94</v>
       </c>
@@ -1487,7 +1554,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>95</v>
       </c>
@@ -1501,10 +1568,10 @@
         <v>90</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1512,10 +1579,10 @@
         <v>95</v>
       </c>
       <c r="C20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>91</v>
@@ -1524,7 +1591,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>97</v>
       </c>
@@ -1549,7 +1616,7 @@
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>97</v>
       </c>
@@ -1574,12 +1641,12 @@
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" t="s">
         <v>80</v>
@@ -1588,47 +1655,47 @@
         <v>110</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>111</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
         <v>113</v>
@@ -1640,138 +1707,138 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
         <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
         <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E28" t="s">
         <v>85</v>
       </c>
       <c r="G28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B29" s="21" t="s">
         <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" t="s">
         <v>86</v>
       </c>
       <c r="G29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" s="21" t="s">
         <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
         <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" s="21" t="s">
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
         <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" s="21" t="s">
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E32" t="s">
         <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="22" t="s">
         <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="20" t="s">
         <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>83</v>
       </c>
       <c r="G34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="20" t="s">
         <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="22" t="s">
         <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>88</v>
@@ -1781,41 +1848,50 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C52:D1048576 C1:D7 C14:D18 D42:D51 C27:D41">
-    <cfRule type="duplicateValues" dxfId="11" priority="29"/>
+  <conditionalFormatting sqref="C52:D1048576 C1:D7 C14:D18 D42:D51 C27:D32 C34:D35 C37:D41">
+    <cfRule type="duplicateValues" dxfId="16" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="duplicateValues" dxfId="10" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="duplicateValues" dxfId="9" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:D20">
-    <cfRule type="duplicateValues" dxfId="8" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:D22">
-    <cfRule type="duplicateValues" dxfId="7" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="duplicateValues" dxfId="6" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="duplicateValues" dxfId="5" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E33">
-    <cfRule type="duplicateValues" dxfId="4" priority="15"/>
+  <conditionalFormatting sqref="E28:E32">
+    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24 G26">
-    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:D33">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:D36">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1823,7 +1899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1833,14 +1909,14 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -1857,7 +1933,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1868,7 +1944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1879,17 +1955,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1903,7 +1979,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1917,7 +1993,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1931,7 +2007,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1945,7 +2021,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1959,7 +2035,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1973,7 +2049,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1987,7 +2063,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2001,7 +2077,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -2015,7 +2091,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2036,15 +2112,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2295,6 +2362,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2308,14 +2384,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2330,6 +2398,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated bodebooks D4_persontime and D4_persontime_Cube
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="146">
   <si>
     <t>status</t>
   </si>
@@ -462,9 +462,6 @@
     <t>D4_persontime_ImmDis</t>
   </si>
   <si>
-    <t>D3_followup_periods_in_cohort_ImmDis D3_flares_ImmDis</t>
-  </si>
-  <si>
     <t>D4_analytical_dataset_KM_ImmDis</t>
   </si>
   <si>
@@ -522,13 +519,22 @@
     <t>05_T4_50_Table_6_components_flares_{ImmDis}</t>
   </si>
   <si>
-    <t xml:space="preserve">D4_components_flare_E_GRAVES_AESI D4_components_flare_Im_HASHIMOTO_AESI D4_components_flare_V_PAN_AESI D4_components_flare_TD_M_ARTRHEU_AESI D4_components_flare_TD_M_ARTPSORIATIC_AESI D4_components_flare_N_DEMYELMS_AESI D4_components_flare_SK_ERYTHEMANODOSUM_AESI D4_components_flare_Im_SLE_AESI D4_components_flare_D_ULCERATIVECOLITIS_AESI D4_components_flare_D_HEPATITISAUTOIMMUNE_AESI </t>
-  </si>
-  <si>
     <t>D5_Table_6_Impact_of_component_flare_ImmDis</t>
   </si>
   <si>
     <t>D5_Table_8_Impact_of_ablation_cohort_ImmDis</t>
+  </si>
+  <si>
+    <t>D3_followup_periods_in_cohort_ImmDis D3_flares_ImmDis D3_PERSONS</t>
+  </si>
+  <si>
+    <t>D4_persontime_Cube_ImmDis</t>
+  </si>
+  <si>
+    <t>04_T3_11_create_persontime_Cube</t>
+  </si>
+  <si>
+    <t>D5_IR</t>
   </si>
 </sst>
 </file>
@@ -682,27 +688,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1168,13 +1154,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,7 +1554,7 @@
         <v>90</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1673,52 +1659,52 @@
         <v>82</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
-        <v>95</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="G25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G27" s="10" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -1726,13 +1712,13 @@
         <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" t="s">
-        <v>85</v>
+        <v>127</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="G28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -1740,13 +1726,13 @@
         <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1754,13 +1740,13 @@
         <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G30" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -1768,13 +1754,13 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
         <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -1782,115 +1768,143 @@
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E32" t="s">
         <v>87</v>
       </c>
       <c r="G32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="C35" t="s">
         <v>140</v>
       </c>
-      <c r="G33" t="s">
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G38" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C52:D1048576 C1:D7 C14:D18 D42:D51 C27:D32 C34:D35 C37:D41">
-    <cfRule type="duplicateValues" dxfId="16" priority="32"/>
+  <conditionalFormatting sqref="C54:D1048576 C1:D7 C14:D18 D44:D53 C28:D34 C36:D37 C39:D43">
+    <cfRule type="duplicateValues" dxfId="14" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="duplicateValues" dxfId="15" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="duplicateValues" dxfId="14" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:D20">
-    <cfRule type="duplicateValues" dxfId="13" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:D22">
-    <cfRule type="duplicateValues" dxfId="12" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G25">
-    <cfRule type="duplicateValues" dxfId="10" priority="19"/>
+  <conditionalFormatting sqref="G26">
+    <cfRule type="duplicateValues" dxfId="8" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E32">
-    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
+  <conditionalFormatting sqref="E29:E34">
+    <cfRule type="duplicateValues" dxfId="7" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="duplicateValues" dxfId="8" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="duplicateValues" dxfId="6" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24 G26">
-    <cfRule type="duplicateValues" dxfId="5" priority="42"/>
+  <conditionalFormatting sqref="G27 G24">
+    <cfRule type="duplicateValues" dxfId="3" priority="42"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:D33">
+  <conditionalFormatting sqref="C35:D35">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E35">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:D36">
+  <conditionalFormatting sqref="C38:D38">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2112,6 +2126,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2362,28 +2397,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2400,29 +2439,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
included number of flares
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="145">
   <si>
     <t>status</t>
   </si>
@@ -532,9 +532,6 @@
   </si>
   <si>
     <t>04_T3_11_create_persontime_Cube</t>
-  </si>
-  <si>
-    <t>D5_IR</t>
   </si>
 </sst>
 </file>
@@ -1154,13 +1151,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1754,7 +1751,7 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E31" t="s">
         <v>87</v>
@@ -1768,7 +1765,7 @@
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E32" t="s">
         <v>87</v>
@@ -1782,41 +1779,41 @@
         <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
         <v>87</v>
       </c>
       <c r="G33" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="21" t="s">
-        <v>94</v>
+      <c r="B34" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="G34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="22" t="s">
-        <v>95</v>
+      <c r="B35" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
@@ -1824,7 +1821,7 @@
         <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>83</v>
@@ -1834,35 +1831,21 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="20" t="s">
-        <v>96</v>
+      <c r="B37" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G38" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C54:D1048576 C1:D7 C14:D18 D44:D53 C28:D34 C36:D37 C39:D43">
+  <conditionalFormatting sqref="C53:D1048576 C1:D7 C14:D18 D43:D52 C28:D33 C35:D36 C38:D42">
     <cfRule type="duplicateValues" dxfId="14" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
@@ -1883,29 +1866,29 @@
   <conditionalFormatting sqref="G26">
     <cfRule type="duplicateValues" dxfId="8" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E34">
-    <cfRule type="duplicateValues" dxfId="7" priority="18"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="duplicateValues" dxfId="6" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="duplicateValues" dxfId="5" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="duplicateValues" dxfId="4" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27 G24">
-    <cfRule type="duplicateValues" dxfId="3" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="42"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:D35">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="C34:D34">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:D38">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C37:D37">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:E33">
+    <cfRule type="duplicateValues" dxfId="0" priority="50"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2126,27 +2109,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2397,32 +2359,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2439,4 +2397,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
merged pregnancy TD in cohort periods
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -15,12 +15,12 @@
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="151">
   <si>
     <t>status</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>03_T2_60_create_pregnancies_during_periods_followup</t>
+  </si>
+  <si>
+    <t>D3_followup_periods_in_cohort_with_pregnancy_ImmDis</t>
+  </si>
+  <si>
+    <t>03_T2_70_create_periods_followup_with_pregnancies</t>
+  </si>
+  <si>
+    <t>D3_followup_periods_in_cohort_ImmDis D3_pregnancy_while_in_followup_periods_in_cohort_ImmDis</t>
   </si>
 </sst>
 </file>
@@ -694,7 +703,17 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1170,13 +1189,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1682,77 +1701,81 @@
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>124</v>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>141</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>94</v>
       </c>
       <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
         <v>126</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1760,13 +1783,13 @@
         <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" t="s">
-        <v>85</v>
+        <v>127</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="G30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -1774,10 +1797,10 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" t="s">
         <v>130</v>
@@ -1788,13 +1811,13 @@
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G32" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
@@ -1802,7 +1825,7 @@
         <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E33" t="s">
         <v>87</v>
@@ -1816,41 +1839,41 @@
         <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
         <v>87</v>
       </c>
       <c r="G34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="22" t="s">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>139</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>144</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
@@ -1858,7 +1881,7 @@
         <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>83</v>
@@ -1868,66 +1891,83 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>140</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C54:D1048576 C1:D7 C14:D18 D44:D53 C29:D34 C36:D37 C39:D43">
-    <cfRule type="duplicateValues" dxfId="15" priority="33"/>
+  <conditionalFormatting sqref="C55:D1048576 C1:D7 C14:D18 D45:D54 C30:D35 C37:D38 C40:D44">
+    <cfRule type="duplicateValues" dxfId="16" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
+    <cfRule type="duplicateValues" dxfId="15" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
     <cfRule type="duplicateValues" dxfId="14" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
+  <conditionalFormatting sqref="C20:D20">
     <cfRule type="duplicateValues" dxfId="13" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:D20">
-    <cfRule type="duplicateValues" dxfId="12" priority="27"/>
+  <conditionalFormatting sqref="C21:D22">
+    <cfRule type="duplicateValues" dxfId="12" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:D22">
+  <conditionalFormatting sqref="G18">
     <cfRule type="duplicateValues" dxfId="11" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="duplicateValues" dxfId="10" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="duplicateValues" dxfId="9" priority="20"/>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="duplicateValues" dxfId="10" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
+    <cfRule type="duplicateValues" dxfId="9" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:C25">
     <cfRule type="duplicateValues" dxfId="8" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C24">
+  <conditionalFormatting sqref="G23">
     <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
-    <cfRule type="duplicateValues" dxfId="6" priority="16"/>
+  <conditionalFormatting sqref="G29 G26">
+    <cfRule type="duplicateValues" dxfId="6" priority="44"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28 G25">
-    <cfRule type="duplicateValues" dxfId="5" priority="43"/>
+  <conditionalFormatting sqref="C36:D36">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:D35">
+  <conditionalFormatting sqref="E36">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
+  <conditionalFormatting sqref="C39:D39">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:D38">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E34">
-    <cfRule type="duplicateValues" dxfId="1" priority="51"/>
+  <conditionalFormatting sqref="E31:E35">
+    <cfRule type="duplicateValues" dxfId="2" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2149,15 +2189,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2412,27 +2449,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2457,9 +2488,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated codebooks and documentation
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="index" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Parameters" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="index" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Parameters" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="171">
   <si>
     <t xml:space="preserve">status</t>
   </si>
@@ -575,6 +575,30 @@
     <t xml:space="preserve">06_T5_80_Table_8_Impact_of_ablation</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Figure_ablation_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ImmDis</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">06_T5_81_Fig_ablation</t>
+  </si>
+  <si>
     <t xml:space="preserve">parameter in the table name</t>
   </si>
   <si>
@@ -687,7 +711,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -732,6 +756,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1219,6 +1249,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1227,14 +1363,14 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="G46" activeCellId="0" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.29"/>
@@ -1493,7 +1629,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1512,7 +1648,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1531,7 +1667,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1550,7 +1686,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1601,7 +1737,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1621,7 +1757,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
         <v>65</v>
       </c>
@@ -1671,7 +1807,7 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1692,7 +1828,7 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
         <v>27</v>
       </c>
@@ -1710,7 +1846,7 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1728,7 +1864,7 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
         <v>27</v>
       </c>
@@ -1746,7 +1882,7 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
@@ -2031,10 +2167,24 @@
         <v>120</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="C55:D1048576 C1:D5 C12:D16 D45:D54 C31:D35 C37:D38 D40 C41:D44">
+  <conditionalFormatting sqref="C55:D1048576 C1:D5 C12:D16 C31:D35 C37:D38 D40 C41:D44 D45:D54">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
@@ -2115,10 +2265,10 @@
   <conditionalFormatting sqref="G44">
     <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
+  <conditionalFormatting sqref="G45:G46">
     <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
+  <conditionalFormatting sqref="C45:C46">
     <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2146,7 +2296,7 @@
       <selection pane="bottomRight" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="62.42"/>
@@ -2155,19 +2305,19 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,179 +2325,179 @@
         <v>23</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change CCD step name to same of script
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -95,7 +95,7 @@
     <t xml:space="preserve">conceptsetdataset</t>
   </si>
   <si>
-    <t xml:space="preserve">01_T2_31_CreateConceptSetDatasets</t>
+    <t xml:space="preserve">01_T2_30_CreateConceptSetDatasets</t>
   </si>
   <si>
     <t xml:space="preserve">g_intermediate/conceptset_datasets</t>
@@ -575,25 +575,7 @@
     <t xml:space="preserve">06_T5_80_Table_8_Impact_of_ablation</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Figure_ablation_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ImmDis</t>
-    </r>
+    <t xml:space="preserve">Figure_ablation_ImmDis</t>
   </si>
   <si>
     <t xml:space="preserve">06_T5_81_Fig_ablation</t>
@@ -711,7 +693,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -756,12 +738,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1367,7 +1343,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="G46" activeCellId="0" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Change step name to 04_T3_30_create_component_dataset
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -470,7 +470,7 @@
     <t xml:space="preserve">analytical dataset for component strategy</t>
   </si>
   <si>
-    <t xml:space="preserve">04_T3_30_create_components_dataset</t>
+    <t xml:space="preserve">04_T3_30_create_component_dataset</t>
   </si>
   <si>
     <t xml:space="preserve">D5_Table_1_Attrition_ImmDis</t>
@@ -1339,11 +1339,11 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>